<commit_message>
Add automatic rotation to the x axis labels
</commit_message>
<xml_diff>
--- a/data_external/data.xlsx
+++ b/data_external/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlillywhite\PyCharmProjects\data_external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE8E7BA-2FF0-40F0-912F-8AC3937AE0EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62CC13D-AA0A-4C81-9B19-A7C9D7AF7BA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="6165" xr2:uid="{1641FD17-90EC-4D7F-AF3B-EEBF340A9990}"/>
   </bookViews>
@@ -38,43 +38,43 @@
     <t>Model Data</t>
   </si>
   <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
     <t>May</t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
     <t>Evap Rate</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A6" sqref="A6:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -453,12 +453,12 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0.3</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0.5</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>2.6</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>3.4</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>3.7</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>2.1</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>0.8</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>0.4</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>0.1</v>

</xml_diff>